<commit_message>
tabs[7] 셀 테두리 적용 (#9)
</commit_message>
<xml_diff>
--- a/templates/template_A.xlsx
+++ b/templates/template_A.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmj\project\__project_original\group_classification\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED4E02A-136E-4358-A546-236CA93F119A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDDF8C8-DE7A-4D0B-8CC6-F74418CD14A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{881DDEE8-C9FF-4D06-99D8-64DA1D3B4EC0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{881DDEE8-C9FF-4D06-99D8-64DA1D3B4EC0}"/>
   </bookViews>
   <sheets>
     <sheet name="설명" sheetId="1" r:id="rId1"/>
@@ -223,7 +223,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -311,13 +311,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -384,40 +399,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -426,8 +426,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -863,14 +881,14 @@
   <sheetData>
     <row r="1" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="35"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -889,77 +907,77 @@
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="27"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="36"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="2:10" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="27"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="36"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="27"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="36"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="27"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="36"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="27"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="36"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="27"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="36"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1102,123 +1120,123 @@
       <c r="B22" s="11"/>
     </row>
     <row r="23" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
       <c r="H23" s="12"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
     <row r="24" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="2:10" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="30"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
       <c r="H27" s="12"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
       <c r="H28" s="13"/>
     </row>
     <row r="29" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
       <c r="H29" s="13"/>
     </row>
     <row r="31" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="34"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="29"/>
     </row>
     <row r="32" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="36"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="24"/>
     </row>
     <row r="33" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="36"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="24"/>
     </row>
     <row r="34" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="36"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="24"/>
     </row>
     <row r="35" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="12"/>
@@ -1283,12 +1301,6 @@
     <row r="48" spans="2:8" s="16" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B33:G33"/>
     <mergeCell ref="B27:G27"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B4:G4"/>
@@ -1301,6 +1313,12 @@
     <mergeCell ref="B24:G24"/>
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1313,35 +1331,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E54A1BC5-FA2F-4626-8785-C8B0327121DF}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="37" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1355,38 +1371,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9BA6FAF-8433-4B01-A3BA-126947EF517C}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="37" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chore : compact 타입 설명 추가
</commit_message>
<xml_diff>
--- a/templates/template_A.xlsx
+++ b/templates/template_A.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmj\project\__project_original\group_classification\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED4E02A-136E-4358-A546-236CA93F119A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A906CA28-F58C-46AC-86CB-CB769AA5823B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{881DDEE8-C9FF-4D06-99D8-64DA1D3B4EC0}"/>
+    <workbookView xWindow="32685" yWindow="1950" windowWidth="17370" windowHeight="13425" xr2:uid="{881DDEE8-C9FF-4D06-99D8-64DA1D3B4EC0}"/>
   </bookViews>
   <sheets>
-    <sheet name="설명" sheetId="1" r:id="rId1"/>
+    <sheet name="설명" sheetId="4" r:id="rId1"/>
     <sheet name="기존반번호순" sheetId="2" r:id="rId2"/>
     <sheet name="신규반번호순" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t> &lt;잠재능력진단검사 A형(능력) 검사 해석 시 유의사항&gt;</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -170,6 +170,42 @@
   </si>
   <si>
     <t>종합지수 P</t>
+  </si>
+  <si>
+    <r>
+      <t> &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>잠재능력진단검사 Compact type 검사 해석 시 유의사항&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">결과 점수는 원점수 그대로가 아니라 표준화된 점수로 제시됩니다. 그러므로 검사 결과를 변환하고 해석할 때, 규준 집단과 피검자의 특성이 완전히 일치하지 않기 때문에, </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>대개 검사 점수에 변동영역이 있을 수 있습니다. 그러므로 검사 결과를 해석할 때 이러한 부분을 고려해, 유연하게 과잉해석을 피하도록 하여야 합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">※ T점수: 평균이 40, 표준편차가 10인 표준 점수로서 50점을 기준으로 이보다 위의 점수는 또래의 평균보다 높고, 이보다 아래 점수는 또래의 평균보다 낮음을 의미합니다. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>※ 백분위: 전체를 100으로 볼 때, 한 개인의 점수가 아래에서부터 몇 번째에 해당하는가를 나타내는 수치입니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 기초학습역량 결과는 7가지 수준(최우수, 매우 우수, 우수, 보통, 낮음, 매우 낮음, 부족)으로 나뉘며, 외향성과 정서적 민감성 결과는 3가지 수준(높음, 보통, 낮음)으로 나뉩니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -215,15 +251,21 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -311,13 +353,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -384,40 +441,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -426,8 +471,65 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,7 +568,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC1380C6-6C8F-45CE-BBFE-1095DD4D71A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA4D3406-5004-4151-817E-AF0482D86DF5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -509,10 +611,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="그림 4">
+        <xdr:cNvPr id="3" name="그림 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F39B241-005E-B5DE-AC41-F13801F5D478}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8BE91BC-FF74-475C-81B4-71658A8457A1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -534,8 +636,97 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="638735" y="8124265"/>
-          <a:ext cx="6916115" cy="4296375"/>
+          <a:off x="638175" y="8162925"/>
+          <a:ext cx="6917796" cy="4299737"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>593912</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>235324</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="그림 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D73CD3BB-39F6-4EF4-98BA-827D3F09BDC1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="638175" y="14782800"/>
+          <a:ext cx="7251887" cy="2959474"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>280148</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>437030</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>190093</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="그림 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15F0516A-D591-464A-B66C-CEB53C20CB19}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:srcRect t="5086"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="518273" y="17540568"/>
+          <a:ext cx="7214907" cy="1890025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -843,12 +1034,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0228A26E-22A4-4172-A883-C1B7BA77BD7C}">
-  <dimension ref="B1:J48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A23AD374-4BB3-4989-BC63-B685AB7DA586}">
+  <dimension ref="B1:J75"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -863,14 +1052,14 @@
   <sheetData>
     <row r="1" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="36"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -889,77 +1078,77 @@
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="27"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="37"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="2:10" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="27"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="37"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="27"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="37"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="27"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="37"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="27"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="37"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="27"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="37"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1115,69 +1304,69 @@
       <c r="J23" s="2"/>
     </row>
     <row r="24" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="2:10" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="30"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
       <c r="H27" s="12"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
       <c r="H28" s="13"/>
     </row>
     <row r="29" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
       <c r="H29" s="13"/>
     </row>
     <row r="31" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1188,37 +1377,37 @@
       <c r="D31" s="29"/>
       <c r="E31" s="29"/>
       <c r="F31" s="29"/>
-      <c r="G31" s="34"/>
+      <c r="G31" s="30"/>
     </row>
     <row r="32" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="36"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="25"/>
     </row>
     <row r="33" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="36"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="25"/>
     </row>
     <row r="34" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="36"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="25"/>
     </row>
     <row r="35" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="12"/>
@@ -1279,16 +1468,185 @@
       <c r="F46" s="19"/>
       <c r="G46" s="20"/>
     </row>
-    <row r="47" spans="2:8" s="16" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="2:8" s="16" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="2:8" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" s="39"/>
+      <c r="D48" s="39"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="39"/>
+      <c r="G48" s="40"/>
+    </row>
+    <row r="49" spans="2:7" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C49" s="41"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="41"/>
+      <c r="G49" s="42"/>
+    </row>
+    <row r="50" spans="2:7" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C50" s="41"/>
+      <c r="D50" s="41"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="41"/>
+      <c r="G50" s="42"/>
+    </row>
+    <row r="51" spans="2:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="13"/>
+      <c r="G51" s="14"/>
+    </row>
+    <row r="52" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="C52" s="44"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
+      <c r="G52" s="45"/>
+    </row>
+    <row r="53" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C53" s="44"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="44"/>
+      <c r="G53" s="45"/>
+    </row>
+    <row r="54" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="44"/>
+      <c r="D54" s="44"/>
+      <c r="E54" s="44"/>
+      <c r="F54" s="44"/>
+      <c r="G54" s="45"/>
+    </row>
+    <row r="55" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="C55" s="47"/>
+      <c r="D55" s="47"/>
+      <c r="E55" s="47"/>
+      <c r="F55" s="47"/>
+      <c r="G55" s="48"/>
+    </row>
+    <row r="56" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="13"/>
+      <c r="G56" s="14"/>
+    </row>
+    <row r="57" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="13"/>
+      <c r="G57" s="14"/>
+    </row>
+    <row r="58" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="13"/>
+      <c r="G58" s="14"/>
+    </row>
+    <row r="59" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="13"/>
+      <c r="G59" s="14"/>
+    </row>
+    <row r="60" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="13"/>
+      <c r="G60" s="14"/>
+    </row>
+    <row r="61" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="13"/>
+      <c r="G61" s="14"/>
+    </row>
+    <row r="62" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="13"/>
+      <c r="G62" s="14"/>
+    </row>
+    <row r="63" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="13"/>
+      <c r="G63" s="14"/>
+    </row>
+    <row r="64" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="13"/>
+      <c r="G64" s="14"/>
+    </row>
+    <row r="65" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="13"/>
+      <c r="G65" s="14"/>
+    </row>
+    <row r="66" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="13"/>
+      <c r="G66" s="14"/>
+    </row>
+    <row r="67" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="13"/>
+      <c r="G67" s="14"/>
+    </row>
+    <row r="68" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="13"/>
+      <c r="G68" s="14"/>
+    </row>
+    <row r="69" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="13"/>
+      <c r="G69" s="14"/>
+    </row>
+    <row r="70" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="13"/>
+      <c r="G70" s="14"/>
+    </row>
+    <row r="71" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="13"/>
+      <c r="G71" s="14"/>
+    </row>
+    <row r="72" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="13"/>
+      <c r="G72" s="14"/>
+    </row>
+    <row r="73" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="13"/>
+      <c r="G73" s="14"/>
+    </row>
+    <row r="74" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="13"/>
+      <c r="G74" s="14"/>
+    </row>
+    <row r="75" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="49"/>
+      <c r="C75" s="50"/>
+      <c r="D75" s="50"/>
+      <c r="E75" s="50"/>
+      <c r="F75" s="50"/>
+      <c r="G75" s="51"/>
+    </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="B34:G34"/>
+  <mergeCells count="25">
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B54:G54"/>
     <mergeCell ref="B28:G28"/>
     <mergeCell ref="B29:G29"/>
     <mergeCell ref="B31:G31"/>
     <mergeCell ref="B32:G32"/>
     <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
     <mergeCell ref="B27:G27"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B4:G4"/>
@@ -1296,11 +1654,6 @@
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1313,35 +1666,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E54A1BC5-FA2F-4626-8785-C8B0327121DF}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="22" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1355,38 +1706,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9BA6FAF-8433-4B01-A3BA-126947EF517C}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="22" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chore : compact 검사 설명 추가
</commit_message>
<xml_diff>
--- a/templates/template_A.xlsx
+++ b/templates/template_A.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmj\project\__project_original\group_classification\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18CE6FE-5B22-4970-B0F1-6E0B1F540A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39165D9D-4C1F-4E49-A1E4-9EC255A0408A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{881DDEE8-C9FF-4D06-99D8-64DA1D3B4EC0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{881DDEE8-C9FF-4D06-99D8-64DA1D3B4EC0}"/>
   </bookViews>
   <sheets>
-    <sheet name="설명" sheetId="1" r:id="rId1"/>
+    <sheet name="설명" sheetId="4" r:id="rId1"/>
     <sheet name="기존반번호순" sheetId="2" r:id="rId2"/>
     <sheet name="신규반번호순" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
   <si>
     <t> &lt;잠재능력진단검사 A형(능력) 검사 해석 시 유의사항&gt;</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -170,6 +170,42 @@
   </si>
   <si>
     <t>종합지수 P</t>
+  </si>
+  <si>
+    <r>
+      <t> &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>잠재능력진단검사 Compact type 검사 해석 시 유의사항&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">결과 점수는 원점수 그대로가 아니라 표준화된 점수로 제시됩니다. 그러므로 검사 결과를 변환하고 해석할 때, 규준 집단과 피검자의 특성이 완전히 일치하지 않기 때문에, </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>대개 검사 점수에 변동영역이 있을 수 있습니다. 그러므로 검사 결과를 해석할 때 이러한 부분을 고려해, 유연하게 과잉해석을 피하도록 하여야 합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">※ T점수: 평균이 40, 표준편차가 10인 표준 점수로서 50점을 기준으로 이보다 위의 점수는 또래의 평균보다 높고, 이보다 아래 점수는 또래의 평균보다 낮음을 의미합니다. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>※ 백분위: 전체를 100으로 볼 때, 한 개인의 점수가 아래에서부터 몇 번째에 해당하는가를 나타내는 수치입니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 기초학습역량 결과는 7가지 수준(최우수, 매우 우수, 우수, 보통, 낮음, 매우 낮음, 부족)으로 나뉘며, 외향성과 정서적 민감성 결과는 3가지 수준(높음, 보통, 낮음)으로 나뉩니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -215,12 +251,18 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -332,7 +374,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -399,43 +441,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -444,8 +471,65 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -484,7 +568,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC1380C6-6C8F-45CE-BBFE-1095DD4D71A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACCDB0D3-5D2A-4516-ADD1-58994BDCAE95}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -527,10 +611,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="그림 4">
+        <xdr:cNvPr id="3" name="그림 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F39B241-005E-B5DE-AC41-F13801F5D478}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6996AB8D-D812-4823-A368-98C365F702B4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -552,8 +636,97 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="638735" y="8124265"/>
-          <a:ext cx="6916115" cy="4296375"/>
+          <a:off x="638175" y="8162925"/>
+          <a:ext cx="6917796" cy="4299737"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>593912</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>235324</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="그림 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C141BD0-9B7E-4D2C-8364-F371574018D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="638175" y="14782800"/>
+          <a:ext cx="7251887" cy="2959474"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>280148</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>437030</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>190093</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="그림 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA4A67C9-8A76-4A8F-AB52-D84939D1B2D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:srcRect t="5086"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="518273" y="17540568"/>
+          <a:ext cx="7214907" cy="1890025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -861,12 +1034,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0228A26E-22A4-4172-A883-C1B7BA77BD7C}">
-  <dimension ref="B1:J48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A27FC6-D95E-40FB-ADD7-3A125311301C}">
+  <dimension ref="B1:J75"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -881,14 +1052,14 @@
   <sheetData>
     <row r="1" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="36"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -907,77 +1078,77 @@
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="27"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="37"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="2:10" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="27"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="37"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="27"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="37"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="27"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="37"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="27"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="37"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="27"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="37"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1133,69 +1304,69 @@
       <c r="J23" s="2"/>
     </row>
     <row r="24" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="2:10" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="30"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
       <c r="H27" s="12"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
       <c r="H28" s="13"/>
     </row>
     <row r="29" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
       <c r="H29" s="13"/>
     </row>
     <row r="31" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1206,37 +1377,37 @@
       <c r="D31" s="29"/>
       <c r="E31" s="29"/>
       <c r="F31" s="29"/>
-      <c r="G31" s="35"/>
+      <c r="G31" s="30"/>
     </row>
     <row r="32" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="32"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="25"/>
     </row>
     <row r="33" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="32"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="25"/>
     </row>
     <row r="34" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="32"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="25"/>
     </row>
     <row r="35" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="12"/>
@@ -1297,16 +1468,185 @@
       <c r="F46" s="19"/>
       <c r="G46" s="20"/>
     </row>
-    <row r="47" spans="2:8" s="16" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="2:8" s="16" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="2:8" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" s="39"/>
+      <c r="D48" s="39"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="39"/>
+      <c r="G48" s="40"/>
+    </row>
+    <row r="49" spans="2:7" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C49" s="41"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="41"/>
+      <c r="G49" s="42"/>
+    </row>
+    <row r="50" spans="2:7" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C50" s="41"/>
+      <c r="D50" s="41"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="41"/>
+      <c r="G50" s="42"/>
+    </row>
+    <row r="51" spans="2:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="13"/>
+      <c r="G51" s="14"/>
+    </row>
+    <row r="52" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="C52" s="44"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
+      <c r="G52" s="45"/>
+    </row>
+    <row r="53" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C53" s="44"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="44"/>
+      <c r="G53" s="45"/>
+    </row>
+    <row r="54" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="44"/>
+      <c r="D54" s="44"/>
+      <c r="E54" s="44"/>
+      <c r="F54" s="44"/>
+      <c r="G54" s="45"/>
+    </row>
+    <row r="55" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="C55" s="47"/>
+      <c r="D55" s="47"/>
+      <c r="E55" s="47"/>
+      <c r="F55" s="47"/>
+      <c r="G55" s="48"/>
+    </row>
+    <row r="56" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="13"/>
+      <c r="G56" s="14"/>
+    </row>
+    <row r="57" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="13"/>
+      <c r="G57" s="14"/>
+    </row>
+    <row r="58" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="13"/>
+      <c r="G58" s="14"/>
+    </row>
+    <row r="59" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="13"/>
+      <c r="G59" s="14"/>
+    </row>
+    <row r="60" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="13"/>
+      <c r="G60" s="14"/>
+    </row>
+    <row r="61" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="13"/>
+      <c r="G61" s="14"/>
+    </row>
+    <row r="62" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="13"/>
+      <c r="G62" s="14"/>
+    </row>
+    <row r="63" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="13"/>
+      <c r="G63" s="14"/>
+    </row>
+    <row r="64" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="13"/>
+      <c r="G64" s="14"/>
+    </row>
+    <row r="65" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="13"/>
+      <c r="G65" s="14"/>
+    </row>
+    <row r="66" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="13"/>
+      <c r="G66" s="14"/>
+    </row>
+    <row r="67" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="13"/>
+      <c r="G67" s="14"/>
+    </row>
+    <row r="68" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="13"/>
+      <c r="G68" s="14"/>
+    </row>
+    <row r="69" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="13"/>
+      <c r="G69" s="14"/>
+    </row>
+    <row r="70" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="13"/>
+      <c r="G70" s="14"/>
+    </row>
+    <row r="71" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="13"/>
+      <c r="G71" s="14"/>
+    </row>
+    <row r="72" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="13"/>
+      <c r="G72" s="14"/>
+    </row>
+    <row r="73" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="13"/>
+      <c r="G73" s="14"/>
+    </row>
+    <row r="74" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="13"/>
+      <c r="G74" s="14"/>
+    </row>
+    <row r="75" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="49"/>
+      <c r="C75" s="50"/>
+      <c r="D75" s="50"/>
+      <c r="E75" s="50"/>
+      <c r="F75" s="50"/>
+      <c r="G75" s="51"/>
+    </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="B34:G34"/>
+  <mergeCells count="25">
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B54:G54"/>
     <mergeCell ref="B28:G28"/>
     <mergeCell ref="B29:G29"/>
     <mergeCell ref="B31:G31"/>
     <mergeCell ref="B32:G32"/>
     <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
     <mergeCell ref="B27:G27"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B4:G4"/>
@@ -1314,11 +1654,6 @@
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1331,33 +1666,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E54A1BC5-FA2F-4626-8785-C8B0327121DF}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="22" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1376,31 +1711,31 @@
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="22" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>